<commit_message>
Lots of refactoring, better calculations and post processing after transfer of amounts - testcases cabin, car, boat, otp,cash,child, crypto and fond is checked out OK
</commit_message>
<xml_diff>
--- a/tests/Feature/config/boat_zero.xlsx
+++ b/tests/Feature/config/boat_zero.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="47">
   <si>
     <t>private</t>
   </si>
@@ -112,7 +112,7 @@
     <t>Anskaffelsesverdi</t>
   </si>
   <si>
-    <t>Betalt (inkl kostnader)</t>
+    <t>Finans kostnader)</t>
   </si>
   <si>
     <t>Skattbar</t>
@@ -148,13 +148,16 @@
     <t>boat</t>
   </si>
   <si>
-    <t xml:space="preserve">000 Asset rule </t>
+    <t xml:space="preserve"> Asset rule: </t>
   </si>
   <si>
-    <t>0Drivstoff/Forsikring/Vedlikehold/Opplagverditap Asset rule Using current amount: 200000 * 1</t>
+    <t>Drivstoff/Forsikring/Vedlikehold/Opplagverditap Asset rule: Using current amount: 200000 * 1</t>
   </si>
   <si>
-    <t>000 Asset rule Using current amount: 200000 * 1</t>
+    <t xml:space="preserve"> Asset rule: Using current amount: 200000 * 1</t>
+  </si>
+  <si>
+    <t>total</t>
   </si>
 </sst>
 </file>
@@ -576,7 +579,7 @@
     <col min="17" max="17" width="6.998" bestFit="true" customWidth="true" style="0"/>
     <col min="18" max="18" width="32.992" bestFit="true" customWidth="true" style="0"/>
     <col min="19" max="19" width="21.138" bestFit="true" customWidth="true" style="0"/>
-    <col min="20" max="20" width="28.136" bestFit="true" customWidth="true" style="0"/>
+    <col min="20" max="20" width="21.138" bestFit="true" customWidth="true" style="0"/>
     <col min="21" max="21" width="15.282" bestFit="true" customWidth="true" style="0"/>
     <col min="22" max="22" width="12.854" bestFit="true" customWidth="true" style="0"/>
     <col min="23" max="23" width="6.998" bestFit="true" customWidth="true" style="0"/>
@@ -808,13 +811,13 @@
       </c>
       <c r="Z6" s="2"/>
       <c r="AA6" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AB6" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AC6" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AD6">
         <v>0</v>
@@ -884,13 +887,13 @@
       </c>
       <c r="Z7" s="2"/>
       <c r="AA7" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AB7" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AC7" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AD7">
         <v>0</v>
@@ -960,13 +963,13 @@
       </c>
       <c r="Z8" s="2"/>
       <c r="AA8" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AB8" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AC8" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AD8">
         <v>0</v>
@@ -1036,13 +1039,13 @@
       </c>
       <c r="Z9" s="2"/>
       <c r="AA9" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AB9" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AC9" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AD9">
         <v>0</v>
@@ -1112,13 +1115,13 @@
       </c>
       <c r="Z10" s="2"/>
       <c r="AA10" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AB10" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AC10" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AD10">
         <v>0</v>
@@ -1188,13 +1191,13 @@
       </c>
       <c r="Z11" s="2"/>
       <c r="AA11" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AB11" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AC11" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AD11">
         <v>0</v>
@@ -1264,13 +1267,13 @@
       </c>
       <c r="Z12" s="2"/>
       <c r="AA12" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AB12" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AC12" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AD12">
         <v>0</v>
@@ -1340,13 +1343,13 @@
       </c>
       <c r="Z13" s="2"/>
       <c r="AA13" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AB13" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AC13" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AD13">
         <v>0</v>
@@ -1416,13 +1419,13 @@
       </c>
       <c r="Z14" s="2"/>
       <c r="AA14" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AB14" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AC14" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AD14">
         <v>0</v>
@@ -1492,13 +1495,13 @@
       </c>
       <c r="Z15" s="2"/>
       <c r="AA15" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AB15" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AC15" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AD15">
         <v>0</v>
@@ -1568,13 +1571,13 @@
       </c>
       <c r="Z16" s="2"/>
       <c r="AA16" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AB16" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AC16" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AD16">
         <v>0</v>
@@ -1644,13 +1647,13 @@
       </c>
       <c r="Z17" s="2"/>
       <c r="AA17" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AB17" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AC17" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AD17">
         <v>0</v>
@@ -1720,13 +1723,13 @@
       </c>
       <c r="Z18" s="2"/>
       <c r="AA18" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AB18" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AC18" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AD18">
         <v>0</v>
@@ -1796,13 +1799,13 @@
       </c>
       <c r="Z19" s="2"/>
       <c r="AA19" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AB19" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AC19" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AD19">
         <v>0</v>
@@ -1872,13 +1875,13 @@
       </c>
       <c r="Z20" s="2"/>
       <c r="AA20" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AB20" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AC20" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AD20">
         <v>0</v>
@@ -1948,13 +1951,13 @@
       </c>
       <c r="Z21" s="2"/>
       <c r="AA21" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AB21" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AC21" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AD21">
         <v>0</v>
@@ -2024,13 +2027,13 @@
       </c>
       <c r="Z22" s="2"/>
       <c r="AA22" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AB22" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AC22" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AD22">
         <v>0</v>
@@ -2100,13 +2103,13 @@
       </c>
       <c r="Z23" s="2"/>
       <c r="AA23" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AB23" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AC23" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AD23">
         <v>0</v>
@@ -2176,13 +2179,13 @@
       </c>
       <c r="Z24" s="2"/>
       <c r="AA24" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AB24" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AC24" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AD24">
         <v>0</v>
@@ -2252,13 +2255,13 @@
       </c>
       <c r="Z25" s="2"/>
       <c r="AA25" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AB25" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AC25" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AD25">
         <v>0</v>
@@ -2328,13 +2331,13 @@
       </c>
       <c r="Z26" s="2"/>
       <c r="AA26" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AB26" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AC26" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AD26">
         <v>0</v>
@@ -2404,13 +2407,13 @@
       </c>
       <c r="Z27" s="2"/>
       <c r="AA27" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AB27" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AC27" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AD27">
         <v>0</v>
@@ -2480,13 +2483,13 @@
       </c>
       <c r="Z28" s="2"/>
       <c r="AA28" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AB28" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AC28" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AD28">
         <v>0</v>
@@ -2556,13 +2559,13 @@
       </c>
       <c r="Z29" s="2"/>
       <c r="AA29" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AB29" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AC29" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AD29">
         <v>0</v>
@@ -2632,13 +2635,13 @@
       </c>
       <c r="Z30" s="2"/>
       <c r="AA30" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AB30" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AC30" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AD30">
         <v>0</v>
@@ -2708,13 +2711,13 @@
       </c>
       <c r="Z31" s="2"/>
       <c r="AA31" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AB31" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AC31" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AD31">
         <v>0</v>
@@ -2784,13 +2787,13 @@
       </c>
       <c r="Z32" s="2"/>
       <c r="AA32" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AB32" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AC32" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AD32">
         <v>0</v>
@@ -2860,13 +2863,13 @@
       </c>
       <c r="Z33" s="2"/>
       <c r="AA33" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AB33" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AC33" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AD33">
         <v>0</v>
@@ -2936,13 +2939,13 @@
       </c>
       <c r="Z34" s="2"/>
       <c r="AA34" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AB34" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AC34" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AD34">
         <v>0</v>
@@ -3012,13 +3015,13 @@
       </c>
       <c r="Z35" s="2"/>
       <c r="AA35" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AB35" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AC35" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AD35">
         <v>0</v>
@@ -3088,13 +3091,13 @@
       </c>
       <c r="Z36" s="2"/>
       <c r="AA36" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AB36" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AC36" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AD36">
         <v>0</v>
@@ -3114,7 +3117,7 @@
       </c>
       <c r="D37" s="2"/>
       <c r="E37" s="5">
-        <v>2000.0</v>
+        <v>24000.0</v>
       </c>
       <c r="F37" s="2"/>
       <c r="G37" s="1">
@@ -3160,17 +3163,17 @@
       </c>
       <c r="X37" s="2"/>
       <c r="Y37" s="1">
-        <v>-2000.0</v>
+        <v>-24000.0</v>
       </c>
       <c r="Z37" s="2"/>
       <c r="AA37" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AB37" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AC37" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AD37">
         <v>0</v>
@@ -3190,7 +3193,7 @@
       </c>
       <c r="D38" s="2"/>
       <c r="E38" s="5">
-        <v>2000.0</v>
+        <v>24000.0</v>
       </c>
       <c r="F38" s="2"/>
       <c r="G38" s="1">
@@ -3236,17 +3239,17 @@
       </c>
       <c r="X38" s="2"/>
       <c r="Y38" s="1">
-        <v>-2000.0</v>
+        <v>-24000.0</v>
       </c>
       <c r="Z38" s="2"/>
       <c r="AA38" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AB38" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AC38" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AD38">
         <v>0</v>
@@ -3266,7 +3269,7 @@
       </c>
       <c r="D39" s="9"/>
       <c r="E39" s="8">
-        <v>2000.0</v>
+        <v>24000.0</v>
       </c>
       <c r="F39" s="9"/>
       <c r="G39" s="8">
@@ -3312,17 +3315,17 @@
       </c>
       <c r="X39" s="9"/>
       <c r="Y39" s="8">
-        <v>-2000.0</v>
+        <v>-24000.0</v>
       </c>
       <c r="Z39" s="9"/>
       <c r="AA39" s="8">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AB39" s="8">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AC39" s="8">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AD39" s="7">
         <v>0</v>
@@ -3343,7 +3346,7 @@
       </c>
       <c r="D40" s="12"/>
       <c r="E40" s="11">
-        <v>2000.0</v>
+        <v>24000.0</v>
       </c>
       <c r="F40" s="12"/>
       <c r="G40" s="11">
@@ -3389,17 +3392,17 @@
       </c>
       <c r="X40" s="12"/>
       <c r="Y40" s="11">
-        <v>-2000.0</v>
+        <v>-24000.0</v>
       </c>
       <c r="Z40" s="12"/>
       <c r="AA40" s="11">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AB40" s="11">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AC40" s="11">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AD40" s="10">
         <v>0</v>
@@ -3420,7 +3423,7 @@
       </c>
       <c r="D41" s="2"/>
       <c r="E41" s="5">
-        <v>2000.0</v>
+        <v>24000.0</v>
       </c>
       <c r="F41" s="2"/>
       <c r="G41" s="1">
@@ -3466,17 +3469,17 @@
       </c>
       <c r="X41" s="2"/>
       <c r="Y41" s="1">
-        <v>-2000.0</v>
+        <v>-24000.0</v>
       </c>
       <c r="Z41" s="2"/>
       <c r="AA41" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AB41" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AC41" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AD41">
         <v>0</v>
@@ -3496,7 +3499,7 @@
       </c>
       <c r="D42" s="2"/>
       <c r="E42" s="5">
-        <v>2000.0</v>
+        <v>24000.0</v>
       </c>
       <c r="F42" s="2"/>
       <c r="G42" s="1">
@@ -3542,17 +3545,17 @@
       </c>
       <c r="X42" s="2"/>
       <c r="Y42" s="1">
-        <v>-2000.0</v>
+        <v>-24000.0</v>
       </c>
       <c r="Z42" s="2"/>
       <c r="AA42" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AB42" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AC42" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AD42">
         <v>0</v>
@@ -3572,7 +3575,7 @@
       </c>
       <c r="D43" s="2"/>
       <c r="E43" s="5">
-        <v>2000.0</v>
+        <v>24000.0</v>
       </c>
       <c r="F43" s="2"/>
       <c r="G43" s="1">
@@ -3618,17 +3621,17 @@
       </c>
       <c r="X43" s="2"/>
       <c r="Y43" s="1">
-        <v>-2000.0</v>
+        <v>-24000.0</v>
       </c>
       <c r="Z43" s="2"/>
       <c r="AA43" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AB43" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AC43" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AD43">
         <v>0</v>
@@ -3648,7 +3651,7 @@
       </c>
       <c r="D44" s="2"/>
       <c r="E44" s="5">
-        <v>2000.0</v>
+        <v>24000.0</v>
       </c>
       <c r="F44" s="2"/>
       <c r="G44" s="1">
@@ -3694,17 +3697,17 @@
       </c>
       <c r="X44" s="2"/>
       <c r="Y44" s="1">
-        <v>-2000.0</v>
+        <v>-24000.0</v>
       </c>
       <c r="Z44" s="2"/>
       <c r="AA44" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AB44" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AC44" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AD44">
         <v>0</v>
@@ -3724,7 +3727,7 @@
       </c>
       <c r="D45" s="2"/>
       <c r="E45" s="5">
-        <v>2000.0</v>
+        <v>24000.0</v>
       </c>
       <c r="F45" s="2"/>
       <c r="G45" s="1">
@@ -3770,17 +3773,17 @@
       </c>
       <c r="X45" s="2"/>
       <c r="Y45" s="1">
-        <v>-2000.0</v>
+        <v>-24000.0</v>
       </c>
       <c r="Z45" s="2"/>
       <c r="AA45" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AB45" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AC45" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AD45">
         <v>0</v>
@@ -3800,7 +3803,7 @@
       </c>
       <c r="D46" s="2"/>
       <c r="E46" s="5">
-        <v>2000.0</v>
+        <v>24000.0</v>
       </c>
       <c r="F46" s="2"/>
       <c r="G46" s="1">
@@ -3846,17 +3849,17 @@
       </c>
       <c r="X46" s="2"/>
       <c r="Y46" s="1">
-        <v>-2000.0</v>
+        <v>-24000.0</v>
       </c>
       <c r="Z46" s="2"/>
       <c r="AA46" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AB46" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AC46" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AD46">
         <v>0</v>
@@ -3876,7 +3879,7 @@
       </c>
       <c r="D47" s="2"/>
       <c r="E47" s="5">
-        <v>2000.0</v>
+        <v>24000.0</v>
       </c>
       <c r="F47" s="2"/>
       <c r="G47" s="1">
@@ -3922,17 +3925,17 @@
       </c>
       <c r="X47" s="2"/>
       <c r="Y47" s="1">
-        <v>-2000.0</v>
+        <v>-24000.0</v>
       </c>
       <c r="Z47" s="2"/>
       <c r="AA47" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AB47" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AC47" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AD47">
         <v>0</v>
@@ -3952,7 +3955,7 @@
       </c>
       <c r="D48" s="2"/>
       <c r="E48" s="5">
-        <v>2000.0</v>
+        <v>24000.0</v>
       </c>
       <c r="F48" s="2"/>
       <c r="G48" s="1">
@@ -3998,17 +4001,17 @@
       </c>
       <c r="X48" s="2"/>
       <c r="Y48" s="1">
-        <v>-2000.0</v>
+        <v>-24000.0</v>
       </c>
       <c r="Z48" s="2"/>
       <c r="AA48" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AB48" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AC48" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AD48">
         <v>0</v>
@@ -4028,7 +4031,7 @@
       </c>
       <c r="D49" s="2"/>
       <c r="E49" s="5">
-        <v>2000.0</v>
+        <v>24000.0</v>
       </c>
       <c r="F49" s="2"/>
       <c r="G49" s="1">
@@ -4074,17 +4077,17 @@
       </c>
       <c r="X49" s="2"/>
       <c r="Y49" s="1">
-        <v>-2000.0</v>
+        <v>-24000.0</v>
       </c>
       <c r="Z49" s="2"/>
       <c r="AA49" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AB49" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AC49" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AD49">
         <v>0</v>
@@ -4104,7 +4107,7 @@
       </c>
       <c r="D50" s="2"/>
       <c r="E50" s="5">
-        <v>2000.0</v>
+        <v>24000.0</v>
       </c>
       <c r="F50" s="2"/>
       <c r="G50" s="1">
@@ -4150,17 +4153,17 @@
       </c>
       <c r="X50" s="2"/>
       <c r="Y50" s="1">
-        <v>-2000.0</v>
+        <v>-24000.0</v>
       </c>
       <c r="Z50" s="2"/>
       <c r="AA50" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AB50" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AC50" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AD50">
         <v>0</v>
@@ -4180,7 +4183,7 @@
       </c>
       <c r="D51" s="2"/>
       <c r="E51" s="5">
-        <v>2000.0</v>
+        <v>24000.0</v>
       </c>
       <c r="F51" s="2"/>
       <c r="G51" s="1">
@@ -4226,17 +4229,17 @@
       </c>
       <c r="X51" s="2"/>
       <c r="Y51" s="1">
-        <v>-2000.0</v>
+        <v>-24000.0</v>
       </c>
       <c r="Z51" s="2"/>
       <c r="AA51" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AB51" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AC51" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AD51">
         <v>0</v>
@@ -4256,7 +4259,7 @@
       </c>
       <c r="D52" s="2"/>
       <c r="E52" s="5">
-        <v>2000.0</v>
+        <v>24000.0</v>
       </c>
       <c r="F52" s="2"/>
       <c r="G52" s="1">
@@ -4302,17 +4305,17 @@
       </c>
       <c r="X52" s="2"/>
       <c r="Y52" s="1">
-        <v>-2000.0</v>
+        <v>-24000.0</v>
       </c>
       <c r="Z52" s="2"/>
       <c r="AA52" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AB52" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AC52" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AD52">
         <v>0</v>
@@ -4332,7 +4335,7 @@
       </c>
       <c r="D53" s="14"/>
       <c r="E53" s="13">
-        <v>2000.0</v>
+        <v>24000.0</v>
       </c>
       <c r="F53" s="14"/>
       <c r="G53" s="13">
@@ -4378,17 +4381,17 @@
       </c>
       <c r="X53" s="14"/>
       <c r="Y53" s="13">
-        <v>-2000.0</v>
+        <v>-24000.0</v>
       </c>
       <c r="Z53" s="14"/>
       <c r="AA53" s="13">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AB53" s="13">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AC53" s="13">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AD53" s="3">
         <v>0</v>
@@ -4409,7 +4412,7 @@
       </c>
       <c r="D54" s="2"/>
       <c r="E54" s="5">
-        <v>2000.0</v>
+        <v>24000.0</v>
       </c>
       <c r="F54" s="2"/>
       <c r="G54" s="1">
@@ -4455,17 +4458,17 @@
       </c>
       <c r="X54" s="2"/>
       <c r="Y54" s="1">
-        <v>-2000.0</v>
+        <v>-24000.0</v>
       </c>
       <c r="Z54" s="2"/>
       <c r="AA54" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AB54" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AC54" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AD54">
         <v>0</v>
@@ -4485,7 +4488,7 @@
       </c>
       <c r="D55" s="2"/>
       <c r="E55" s="5">
-        <v>2000.0</v>
+        <v>24000.0</v>
       </c>
       <c r="F55" s="2"/>
       <c r="G55" s="1">
@@ -4531,17 +4534,17 @@
       </c>
       <c r="X55" s="2"/>
       <c r="Y55" s="1">
-        <v>-2000.0</v>
+        <v>-24000.0</v>
       </c>
       <c r="Z55" s="2"/>
       <c r="AA55" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AB55" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AC55" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AD55">
         <v>0</v>
@@ -4561,7 +4564,7 @@
       </c>
       <c r="D56" s="2"/>
       <c r="E56" s="5">
-        <v>2000.0</v>
+        <v>24000.0</v>
       </c>
       <c r="F56" s="2"/>
       <c r="G56" s="1">
@@ -4607,17 +4610,17 @@
       </c>
       <c r="X56" s="2"/>
       <c r="Y56" s="1">
-        <v>-2000.0</v>
+        <v>-24000.0</v>
       </c>
       <c r="Z56" s="2"/>
       <c r="AA56" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AB56" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AC56" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AD56">
         <v>0</v>
@@ -4637,7 +4640,7 @@
       </c>
       <c r="D57" s="14"/>
       <c r="E57" s="13">
-        <v>2000.0</v>
+        <v>24000.0</v>
       </c>
       <c r="F57" s="14"/>
       <c r="G57" s="13">
@@ -4683,17 +4686,17 @@
       </c>
       <c r="X57" s="14"/>
       <c r="Y57" s="13">
-        <v>-2000.0</v>
+        <v>-24000.0</v>
       </c>
       <c r="Z57" s="14"/>
       <c r="AA57" s="13">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AB57" s="13">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AC57" s="13">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AD57" s="3">
         <v>0</v>
@@ -4714,7 +4717,7 @@
       </c>
       <c r="D58" s="2"/>
       <c r="E58" s="5">
-        <v>2000.0</v>
+        <v>24000.0</v>
       </c>
       <c r="F58" s="2"/>
       <c r="G58" s="1">
@@ -4760,17 +4763,17 @@
       </c>
       <c r="X58" s="2"/>
       <c r="Y58" s="1">
-        <v>-2000.0</v>
+        <v>-24000.0</v>
       </c>
       <c r="Z58" s="2"/>
       <c r="AA58" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AB58" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AC58" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AD58">
         <v>0</v>
@@ -4790,7 +4793,7 @@
       </c>
       <c r="D59" s="2"/>
       <c r="E59" s="5">
-        <v>2000.0</v>
+        <v>24000.0</v>
       </c>
       <c r="F59" s="2"/>
       <c r="G59" s="1">
@@ -4836,17 +4839,17 @@
       </c>
       <c r="X59" s="2"/>
       <c r="Y59" s="1">
-        <v>-2000.0</v>
+        <v>-24000.0</v>
       </c>
       <c r="Z59" s="2"/>
       <c r="AA59" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AB59" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AC59" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AD59">
         <v>0</v>
@@ -4866,7 +4869,7 @@
       </c>
       <c r="D60" s="2"/>
       <c r="E60" s="5">
-        <v>2000.0</v>
+        <v>24000.0</v>
       </c>
       <c r="F60" s="2"/>
       <c r="G60" s="1">
@@ -4912,17 +4915,17 @@
       </c>
       <c r="X60" s="2"/>
       <c r="Y60" s="1">
-        <v>-2000.0</v>
+        <v>-24000.0</v>
       </c>
       <c r="Z60" s="2"/>
       <c r="AA60" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AB60" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AC60" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AD60">
         <v>0</v>
@@ -4942,7 +4945,7 @@
       </c>
       <c r="D61" s="2"/>
       <c r="E61" s="5">
-        <v>2000.0</v>
+        <v>24000.0</v>
       </c>
       <c r="F61" s="2"/>
       <c r="G61" s="1">
@@ -4988,17 +4991,17 @@
       </c>
       <c r="X61" s="2"/>
       <c r="Y61" s="1">
-        <v>-2000.0</v>
+        <v>-24000.0</v>
       </c>
       <c r="Z61" s="2"/>
       <c r="AA61" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AB61" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AC61" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AD61">
         <v>0</v>
@@ -5018,7 +5021,7 @@
       </c>
       <c r="D62" s="2"/>
       <c r="E62" s="5">
-        <v>2000.0</v>
+        <v>24000.0</v>
       </c>
       <c r="F62" s="2"/>
       <c r="G62" s="1">
@@ -5064,17 +5067,17 @@
       </c>
       <c r="X62" s="2"/>
       <c r="Y62" s="1">
-        <v>-2000.0</v>
+        <v>-24000.0</v>
       </c>
       <c r="Z62" s="2"/>
       <c r="AA62" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AB62" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AC62" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AD62">
         <v>0</v>
@@ -5094,7 +5097,7 @@
       </c>
       <c r="D63" s="2"/>
       <c r="E63" s="5">
-        <v>2000.0</v>
+        <v>24000.0</v>
       </c>
       <c r="F63" s="2"/>
       <c r="G63" s="1">
@@ -5140,17 +5143,17 @@
       </c>
       <c r="X63" s="2"/>
       <c r="Y63" s="1">
-        <v>-2000.0</v>
+        <v>-24000.0</v>
       </c>
       <c r="Z63" s="2"/>
       <c r="AA63" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AB63" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AC63" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AD63">
         <v>0</v>
@@ -5170,7 +5173,7 @@
       </c>
       <c r="D64" s="2"/>
       <c r="E64" s="5">
-        <v>2000.0</v>
+        <v>24000.0</v>
       </c>
       <c r="F64" s="2"/>
       <c r="G64" s="1">
@@ -5216,17 +5219,17 @@
       </c>
       <c r="X64" s="2"/>
       <c r="Y64" s="1">
-        <v>-2000.0</v>
+        <v>-24000.0</v>
       </c>
       <c r="Z64" s="2"/>
       <c r="AA64" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AB64" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AC64" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AD64">
         <v>0</v>
@@ -5246,7 +5249,7 @@
       </c>
       <c r="D65" s="2"/>
       <c r="E65" s="5">
-        <v>2000.0</v>
+        <v>24000.0</v>
       </c>
       <c r="F65" s="2"/>
       <c r="G65" s="1">
@@ -5292,17 +5295,17 @@
       </c>
       <c r="X65" s="2"/>
       <c r="Y65" s="1">
-        <v>-2000.0</v>
+        <v>-24000.0</v>
       </c>
       <c r="Z65" s="2"/>
       <c r="AA65" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AB65" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AC65" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AD65">
         <v>0</v>
@@ -5322,7 +5325,7 @@
       </c>
       <c r="D66" s="2"/>
       <c r="E66" s="5">
-        <v>2000.0</v>
+        <v>24000.0</v>
       </c>
       <c r="F66" s="2"/>
       <c r="G66" s="1">
@@ -5368,17 +5371,17 @@
       </c>
       <c r="X66" s="2"/>
       <c r="Y66" s="1">
-        <v>-2000.0</v>
+        <v>-24000.0</v>
       </c>
       <c r="Z66" s="2"/>
       <c r="AA66" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AB66" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AC66" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AD66">
         <v>0</v>
@@ -5398,7 +5401,7 @@
       </c>
       <c r="D67" s="2"/>
       <c r="E67" s="5">
-        <v>2000.0</v>
+        <v>24000.0</v>
       </c>
       <c r="F67" s="2"/>
       <c r="G67" s="1">
@@ -5444,17 +5447,17 @@
       </c>
       <c r="X67" s="2"/>
       <c r="Y67" s="1">
-        <v>-2000.0</v>
+        <v>-24000.0</v>
       </c>
       <c r="Z67" s="2"/>
       <c r="AA67" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AB67" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AC67" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AD67">
         <v>0</v>
@@ -5474,7 +5477,7 @@
       </c>
       <c r="D68" s="2"/>
       <c r="E68" s="5">
-        <v>2000.0</v>
+        <v>24000.0</v>
       </c>
       <c r="F68" s="2"/>
       <c r="G68" s="1">
@@ -5520,17 +5523,17 @@
       </c>
       <c r="X68" s="2"/>
       <c r="Y68" s="1">
-        <v>-2000.0</v>
+        <v>-24000.0</v>
       </c>
       <c r="Z68" s="2"/>
       <c r="AA68" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AB68" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AC68" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AD68">
         <v>0</v>
@@ -5550,7 +5553,7 @@
       </c>
       <c r="D69" s="2"/>
       <c r="E69" s="5">
-        <v>2000.0</v>
+        <v>24000.0</v>
       </c>
       <c r="F69" s="2"/>
       <c r="G69" s="1">
@@ -5596,17 +5599,17 @@
       </c>
       <c r="X69" s="2"/>
       <c r="Y69" s="1">
-        <v>-2000.0</v>
+        <v>-24000.0</v>
       </c>
       <c r="Z69" s="2"/>
       <c r="AA69" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AB69" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AC69" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AD69">
         <v>0</v>
@@ -5626,7 +5629,7 @@
       </c>
       <c r="D70" s="2"/>
       <c r="E70" s="5">
-        <v>2000.0</v>
+        <v>24000.0</v>
       </c>
       <c r="F70" s="2"/>
       <c r="G70" s="1">
@@ -5672,17 +5675,17 @@
       </c>
       <c r="X70" s="2"/>
       <c r="Y70" s="1">
-        <v>-2000.0</v>
+        <v>-24000.0</v>
       </c>
       <c r="Z70" s="2"/>
       <c r="AA70" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AB70" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AC70" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AD70">
         <v>0</v>
@@ -5702,7 +5705,7 @@
       </c>
       <c r="D71" s="2"/>
       <c r="E71" s="5">
-        <v>2000.0</v>
+        <v>24000.0</v>
       </c>
       <c r="F71" s="2"/>
       <c r="G71" s="1">
@@ -5748,17 +5751,17 @@
       </c>
       <c r="X71" s="2"/>
       <c r="Y71" s="1">
-        <v>-2000.0</v>
+        <v>-24000.0</v>
       </c>
       <c r="Z71" s="2"/>
       <c r="AA71" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AB71" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AC71" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AD71">
         <v>0</v>
@@ -5778,7 +5781,7 @@
       </c>
       <c r="D72" s="16"/>
       <c r="E72" s="5">
-        <v>2000.0</v>
+        <v>24000.0</v>
       </c>
       <c r="F72" s="16"/>
       <c r="G72" s="5">
@@ -5824,17 +5827,17 @@
       </c>
       <c r="X72" s="16"/>
       <c r="Y72" s="5">
-        <v>-2000.0</v>
+        <v>-24000.0</v>
       </c>
       <c r="Z72" s="16"/>
       <c r="AA72" s="5">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AB72" s="5">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AC72" s="5">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AD72" s="15">
         <v>0</v>
@@ -6131,7 +6134,7 @@
     <col min="17" max="17" width="6.998" bestFit="true" customWidth="true" style="0"/>
     <col min="18" max="18" width="32.992" bestFit="true" customWidth="true" style="0"/>
     <col min="19" max="19" width="21.138" bestFit="true" customWidth="true" style="0"/>
-    <col min="20" max="20" width="28.136" bestFit="true" customWidth="true" style="0"/>
+    <col min="20" max="20" width="21.138" bestFit="true" customWidth="true" style="0"/>
     <col min="21" max="21" width="15.282" bestFit="true" customWidth="true" style="0"/>
     <col min="22" max="22" width="12.854" bestFit="true" customWidth="true" style="0"/>
     <col min="23" max="23" width="6.998" bestFit="true" customWidth="true" style="0"/>
@@ -6347,7 +6350,7 @@
       </c>
       <c r="V6" s="2"/>
       <c r="W6" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="X6" s="2"/>
       <c r="Y6" s="1">
@@ -6355,13 +6358,13 @@
       </c>
       <c r="Z6" s="2"/>
       <c r="AA6" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AB6" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AC6" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AD6">
         <v>0</v>
@@ -6415,7 +6418,7 @@
       </c>
       <c r="V7" s="2"/>
       <c r="W7" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="X7" s="2"/>
       <c r="Y7" s="1">
@@ -6423,13 +6426,13 @@
       </c>
       <c r="Z7" s="2"/>
       <c r="AA7" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AB7" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AC7" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AD7">
         <v>0</v>
@@ -6483,7 +6486,7 @@
       </c>
       <c r="V8" s="2"/>
       <c r="W8" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="X8" s="2"/>
       <c r="Y8" s="1">
@@ -6491,13 +6494,13 @@
       </c>
       <c r="Z8" s="2"/>
       <c r="AA8" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AB8" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AC8" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AD8">
         <v>0</v>
@@ -6551,7 +6554,7 @@
       </c>
       <c r="V9" s="2"/>
       <c r="W9" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="X9" s="2"/>
       <c r="Y9" s="1">
@@ -6559,13 +6562,13 @@
       </c>
       <c r="Z9" s="2"/>
       <c r="AA9" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AB9" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AC9" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AD9">
         <v>0</v>
@@ -6619,7 +6622,7 @@
       </c>
       <c r="V10" s="2"/>
       <c r="W10" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="X10" s="2"/>
       <c r="Y10" s="1">
@@ -6627,13 +6630,13 @@
       </c>
       <c r="Z10" s="2"/>
       <c r="AA10" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AB10" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AC10" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AD10">
         <v>0</v>
@@ -6687,7 +6690,7 @@
       </c>
       <c r="V11" s="2"/>
       <c r="W11" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="X11" s="2"/>
       <c r="Y11" s="1">
@@ -6695,13 +6698,13 @@
       </c>
       <c r="Z11" s="2"/>
       <c r="AA11" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AB11" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AC11" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AD11">
         <v>0</v>
@@ -6755,7 +6758,7 @@
       </c>
       <c r="V12" s="2"/>
       <c r="W12" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="X12" s="2"/>
       <c r="Y12" s="1">
@@ -6763,13 +6766,13 @@
       </c>
       <c r="Z12" s="2"/>
       <c r="AA12" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AB12" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AC12" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AD12">
         <v>0</v>
@@ -6823,7 +6826,7 @@
       </c>
       <c r="V13" s="2"/>
       <c r="W13" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="X13" s="2"/>
       <c r="Y13" s="1">
@@ -6831,13 +6834,13 @@
       </c>
       <c r="Z13" s="2"/>
       <c r="AA13" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AB13" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AC13" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AD13">
         <v>0</v>
@@ -6891,7 +6894,7 @@
       </c>
       <c r="V14" s="2"/>
       <c r="W14" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="X14" s="2"/>
       <c r="Y14" s="1">
@@ -6899,13 +6902,13 @@
       </c>
       <c r="Z14" s="2"/>
       <c r="AA14" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AB14" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AC14" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AD14">
         <v>0</v>
@@ -6959,7 +6962,7 @@
       </c>
       <c r="V15" s="2"/>
       <c r="W15" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="X15" s="2"/>
       <c r="Y15" s="1">
@@ -6967,13 +6970,13 @@
       </c>
       <c r="Z15" s="2"/>
       <c r="AA15" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AB15" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AC15" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AD15">
         <v>0</v>
@@ -7027,7 +7030,7 @@
       </c>
       <c r="V16" s="2"/>
       <c r="W16" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="X16" s="2"/>
       <c r="Y16" s="1">
@@ -7035,13 +7038,13 @@
       </c>
       <c r="Z16" s="2"/>
       <c r="AA16" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AB16" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AC16" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AD16">
         <v>0</v>
@@ -7095,7 +7098,7 @@
       </c>
       <c r="V17" s="2"/>
       <c r="W17" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="X17" s="2"/>
       <c r="Y17" s="1">
@@ -7103,13 +7106,13 @@
       </c>
       <c r="Z17" s="2"/>
       <c r="AA17" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AB17" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AC17" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AD17">
         <v>0</v>
@@ -7163,7 +7166,7 @@
       </c>
       <c r="V18" s="2"/>
       <c r="W18" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="X18" s="2"/>
       <c r="Y18" s="1">
@@ -7171,13 +7174,13 @@
       </c>
       <c r="Z18" s="2"/>
       <c r="AA18" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AB18" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AC18" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AD18">
         <v>0</v>
@@ -7231,7 +7234,7 @@
       </c>
       <c r="V19" s="2"/>
       <c r="W19" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="X19" s="2"/>
       <c r="Y19" s="1">
@@ -7239,13 +7242,13 @@
       </c>
       <c r="Z19" s="2"/>
       <c r="AA19" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AB19" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AC19" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AD19">
         <v>0</v>
@@ -7299,7 +7302,7 @@
       </c>
       <c r="V20" s="2"/>
       <c r="W20" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="X20" s="2"/>
       <c r="Y20" s="1">
@@ -7307,13 +7310,13 @@
       </c>
       <c r="Z20" s="2"/>
       <c r="AA20" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AB20" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AC20" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AD20">
         <v>0</v>
@@ -7367,7 +7370,7 @@
       </c>
       <c r="V21" s="2"/>
       <c r="W21" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="X21" s="2"/>
       <c r="Y21" s="1">
@@ -7375,13 +7378,13 @@
       </c>
       <c r="Z21" s="2"/>
       <c r="AA21" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AB21" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AC21" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AD21">
         <v>0</v>
@@ -7435,7 +7438,7 @@
       </c>
       <c r="V22" s="2"/>
       <c r="W22" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="X22" s="2"/>
       <c r="Y22" s="1">
@@ -7443,13 +7446,13 @@
       </c>
       <c r="Z22" s="2"/>
       <c r="AA22" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AB22" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AC22" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AD22">
         <v>0</v>
@@ -7503,7 +7506,7 @@
       </c>
       <c r="V23" s="2"/>
       <c r="W23" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="X23" s="2"/>
       <c r="Y23" s="1">
@@ -7511,13 +7514,13 @@
       </c>
       <c r="Z23" s="2"/>
       <c r="AA23" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AB23" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AC23" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AD23">
         <v>0</v>
@@ -7571,7 +7574,7 @@
       </c>
       <c r="V24" s="2"/>
       <c r="W24" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="X24" s="2"/>
       <c r="Y24" s="1">
@@ -7579,13 +7582,13 @@
       </c>
       <c r="Z24" s="2"/>
       <c r="AA24" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AB24" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AC24" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AD24">
         <v>0</v>
@@ -7639,7 +7642,7 @@
       </c>
       <c r="V25" s="2"/>
       <c r="W25" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="X25" s="2"/>
       <c r="Y25" s="1">
@@ -7647,13 +7650,13 @@
       </c>
       <c r="Z25" s="2"/>
       <c r="AA25" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AB25" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AC25" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AD25">
         <v>0</v>
@@ -7707,7 +7710,7 @@
       </c>
       <c r="V26" s="2"/>
       <c r="W26" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="X26" s="2"/>
       <c r="Y26" s="1">
@@ -7715,13 +7718,13 @@
       </c>
       <c r="Z26" s="2"/>
       <c r="AA26" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AB26" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AC26" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AD26">
         <v>0</v>
@@ -7775,7 +7778,7 @@
       </c>
       <c r="V27" s="2"/>
       <c r="W27" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="X27" s="2"/>
       <c r="Y27" s="1">
@@ -7783,13 +7786,13 @@
       </c>
       <c r="Z27" s="2"/>
       <c r="AA27" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AB27" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AC27" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AD27">
         <v>0</v>
@@ -7843,7 +7846,7 @@
       </c>
       <c r="V28" s="2"/>
       <c r="W28" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="X28" s="2"/>
       <c r="Y28" s="1">
@@ -7851,13 +7854,13 @@
       </c>
       <c r="Z28" s="2"/>
       <c r="AA28" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AB28" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AC28" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AD28">
         <v>0</v>
@@ -7911,7 +7914,7 @@
       </c>
       <c r="V29" s="2"/>
       <c r="W29" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="X29" s="2"/>
       <c r="Y29" s="1">
@@ -7919,13 +7922,13 @@
       </c>
       <c r="Z29" s="2"/>
       <c r="AA29" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AB29" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AC29" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AD29">
         <v>0</v>
@@ -7979,7 +7982,7 @@
       </c>
       <c r="V30" s="2"/>
       <c r="W30" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="X30" s="2"/>
       <c r="Y30" s="1">
@@ -7987,13 +7990,13 @@
       </c>
       <c r="Z30" s="2"/>
       <c r="AA30" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AB30" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AC30" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AD30">
         <v>0</v>
@@ -8047,7 +8050,7 @@
       </c>
       <c r="V31" s="2"/>
       <c r="W31" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="X31" s="2"/>
       <c r="Y31" s="1">
@@ -8055,13 +8058,13 @@
       </c>
       <c r="Z31" s="2"/>
       <c r="AA31" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AB31" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AC31" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AD31">
         <v>0</v>
@@ -8115,7 +8118,7 @@
       </c>
       <c r="V32" s="2"/>
       <c r="W32" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="X32" s="2"/>
       <c r="Y32" s="1">
@@ -8123,13 +8126,13 @@
       </c>
       <c r="Z32" s="2"/>
       <c r="AA32" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AB32" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AC32" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AD32">
         <v>0</v>
@@ -8183,7 +8186,7 @@
       </c>
       <c r="V33" s="2"/>
       <c r="W33" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="X33" s="2"/>
       <c r="Y33" s="1">
@@ -8191,13 +8194,13 @@
       </c>
       <c r="Z33" s="2"/>
       <c r="AA33" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AB33" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AC33" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AD33">
         <v>0</v>
@@ -8251,7 +8254,7 @@
       </c>
       <c r="V34" s="2"/>
       <c r="W34" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="X34" s="2"/>
       <c r="Y34" s="1">
@@ -8259,13 +8262,13 @@
       </c>
       <c r="Z34" s="2"/>
       <c r="AA34" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AB34" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AC34" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AD34">
         <v>0</v>
@@ -8319,7 +8322,7 @@
       </c>
       <c r="V35" s="2"/>
       <c r="W35" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="X35" s="2"/>
       <c r="Y35" s="1">
@@ -8327,13 +8330,13 @@
       </c>
       <c r="Z35" s="2"/>
       <c r="AA35" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AB35" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AC35" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AD35">
         <v>0</v>
@@ -8387,7 +8390,7 @@
       </c>
       <c r="V36" s="2"/>
       <c r="W36" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="X36" s="2"/>
       <c r="Y36" s="1">
@@ -8395,13 +8398,13 @@
       </c>
       <c r="Z36" s="2"/>
       <c r="AA36" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AB36" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AC36" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AD36">
         <v>0</v>
@@ -8423,7 +8426,7 @@
       </c>
       <c r="D37" s="2"/>
       <c r="E37" s="5">
-        <v>2000.0</v>
+        <v>24000.0</v>
       </c>
       <c r="F37" s="2"/>
       <c r="G37" s="1">
@@ -8457,23 +8460,23 @@
         <v>1</v>
       </c>
       <c r="W37" s="1">
-        <v>2000.0</v>
+        <v>0</v>
       </c>
       <c r="X37" s="2">
         <v>0.01</v>
       </c>
       <c r="Y37" s="1">
-        <v>-2000.0</v>
+        <v>-24000.0</v>
       </c>
       <c r="Z37" s="2"/>
       <c r="AA37" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AB37" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AC37" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AD37">
         <v>0</v>
@@ -8495,7 +8498,7 @@
       </c>
       <c r="D38" s="2"/>
       <c r="E38" s="5">
-        <v>2000.0</v>
+        <v>24000.0</v>
       </c>
       <c r="F38" s="2"/>
       <c r="G38" s="1">
@@ -8529,23 +8532,23 @@
         <v>1</v>
       </c>
       <c r="W38" s="1">
-        <v>2000.0</v>
+        <v>0</v>
       </c>
       <c r="X38" s="2">
         <v>0.01</v>
       </c>
       <c r="Y38" s="1">
-        <v>-2000.0</v>
+        <v>-24000.0</v>
       </c>
       <c r="Z38" s="2"/>
       <c r="AA38" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AB38" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AC38" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AD38">
         <v>0</v>
@@ -8567,7 +8570,7 @@
       </c>
       <c r="D39" s="9"/>
       <c r="E39" s="8">
-        <v>2000.0</v>
+        <v>24000.0</v>
       </c>
       <c r="F39" s="9"/>
       <c r="G39" s="8">
@@ -8601,23 +8604,23 @@
         <v>1</v>
       </c>
       <c r="W39" s="8">
-        <v>2000.0</v>
+        <v>0</v>
       </c>
       <c r="X39" s="9">
         <v>0.01</v>
       </c>
       <c r="Y39" s="8">
-        <v>-2000.0</v>
+        <v>-24000.0</v>
       </c>
       <c r="Z39" s="9"/>
       <c r="AA39" s="8">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AB39" s="8">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AC39" s="8">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AD39" s="7">
         <v>0</v>
@@ -8640,7 +8643,7 @@
       </c>
       <c r="D40" s="12"/>
       <c r="E40" s="11">
-        <v>2000.0</v>
+        <v>24000.0</v>
       </c>
       <c r="F40" s="12"/>
       <c r="G40" s="11">
@@ -8674,23 +8677,23 @@
         <v>1</v>
       </c>
       <c r="W40" s="11">
-        <v>2000.0</v>
+        <v>0</v>
       </c>
       <c r="X40" s="12">
         <v>0.01</v>
       </c>
       <c r="Y40" s="11">
-        <v>-2000.0</v>
+        <v>-24000.0</v>
       </c>
       <c r="Z40" s="12"/>
       <c r="AA40" s="11">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AB40" s="11">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AC40" s="11">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AD40" s="10">
         <v>0</v>
@@ -8713,7 +8716,7 @@
       </c>
       <c r="D41" s="2"/>
       <c r="E41" s="5">
-        <v>2000.0</v>
+        <v>24000.0</v>
       </c>
       <c r="F41" s="2"/>
       <c r="G41" s="1">
@@ -8747,23 +8750,23 @@
         <v>1</v>
       </c>
       <c r="W41" s="1">
-        <v>2000.0</v>
+        <v>0</v>
       </c>
       <c r="X41" s="2">
         <v>0.01</v>
       </c>
       <c r="Y41" s="1">
-        <v>-2000.0</v>
+        <v>-24000.0</v>
       </c>
       <c r="Z41" s="2"/>
       <c r="AA41" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AB41" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AC41" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AD41">
         <v>0</v>
@@ -8785,7 +8788,7 @@
       </c>
       <c r="D42" s="2"/>
       <c r="E42" s="5">
-        <v>2000.0</v>
+        <v>24000.0</v>
       </c>
       <c r="F42" s="2"/>
       <c r="G42" s="1">
@@ -8819,23 +8822,23 @@
         <v>1</v>
       </c>
       <c r="W42" s="1">
-        <v>2000.0</v>
+        <v>0</v>
       </c>
       <c r="X42" s="2">
         <v>0.01</v>
       </c>
       <c r="Y42" s="1">
-        <v>-2000.0</v>
+        <v>-24000.0</v>
       </c>
       <c r="Z42" s="2"/>
       <c r="AA42" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AB42" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AC42" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AD42">
         <v>0</v>
@@ -8857,7 +8860,7 @@
       </c>
       <c r="D43" s="2"/>
       <c r="E43" s="5">
-        <v>2000.0</v>
+        <v>24000.0</v>
       </c>
       <c r="F43" s="2"/>
       <c r="G43" s="1">
@@ -8891,23 +8894,23 @@
         <v>1</v>
       </c>
       <c r="W43" s="1">
-        <v>2000.0</v>
+        <v>0</v>
       </c>
       <c r="X43" s="2">
         <v>0.01</v>
       </c>
       <c r="Y43" s="1">
-        <v>-2000.0</v>
+        <v>-24000.0</v>
       </c>
       <c r="Z43" s="2"/>
       <c r="AA43" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AB43" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AC43" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AD43">
         <v>0</v>
@@ -8929,7 +8932,7 @@
       </c>
       <c r="D44" s="2"/>
       <c r="E44" s="5">
-        <v>2000.0</v>
+        <v>24000.0</v>
       </c>
       <c r="F44" s="2"/>
       <c r="G44" s="1">
@@ -8963,23 +8966,23 @@
         <v>1</v>
       </c>
       <c r="W44" s="1">
-        <v>2000.0</v>
+        <v>0</v>
       </c>
       <c r="X44" s="2">
         <v>0.01</v>
       </c>
       <c r="Y44" s="1">
-        <v>-2000.0</v>
+        <v>-24000.0</v>
       </c>
       <c r="Z44" s="2"/>
       <c r="AA44" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AB44" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AC44" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AD44">
         <v>0</v>
@@ -9001,7 +9004,7 @@
       </c>
       <c r="D45" s="2"/>
       <c r="E45" s="5">
-        <v>2000.0</v>
+        <v>24000.0</v>
       </c>
       <c r="F45" s="2"/>
       <c r="G45" s="1">
@@ -9035,23 +9038,23 @@
         <v>1</v>
       </c>
       <c r="W45" s="1">
-        <v>2000.0</v>
+        <v>0</v>
       </c>
       <c r="X45" s="2">
         <v>0.01</v>
       </c>
       <c r="Y45" s="1">
-        <v>-2000.0</v>
+        <v>-24000.0</v>
       </c>
       <c r="Z45" s="2"/>
       <c r="AA45" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AB45" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AC45" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AD45">
         <v>0</v>
@@ -9073,7 +9076,7 @@
       </c>
       <c r="D46" s="2"/>
       <c r="E46" s="5">
-        <v>2000.0</v>
+        <v>24000.0</v>
       </c>
       <c r="F46" s="2"/>
       <c r="G46" s="1">
@@ -9107,23 +9110,23 @@
         <v>1</v>
       </c>
       <c r="W46" s="1">
-        <v>2000.0</v>
+        <v>0</v>
       </c>
       <c r="X46" s="2">
         <v>0.01</v>
       </c>
       <c r="Y46" s="1">
-        <v>-2000.0</v>
+        <v>-24000.0</v>
       </c>
       <c r="Z46" s="2"/>
       <c r="AA46" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AB46" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AC46" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AD46">
         <v>0</v>
@@ -9145,7 +9148,7 @@
       </c>
       <c r="D47" s="2"/>
       <c r="E47" s="5">
-        <v>2000.0</v>
+        <v>24000.0</v>
       </c>
       <c r="F47" s="2"/>
       <c r="G47" s="1">
@@ -9179,23 +9182,23 @@
         <v>1</v>
       </c>
       <c r="W47" s="1">
-        <v>2000.0</v>
+        <v>0</v>
       </c>
       <c r="X47" s="2">
         <v>0.01</v>
       </c>
       <c r="Y47" s="1">
-        <v>-2000.0</v>
+        <v>-24000.0</v>
       </c>
       <c r="Z47" s="2"/>
       <c r="AA47" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AB47" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AC47" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AD47">
         <v>0</v>
@@ -9217,7 +9220,7 @@
       </c>
       <c r="D48" s="2"/>
       <c r="E48" s="5">
-        <v>2000.0</v>
+        <v>24000.0</v>
       </c>
       <c r="F48" s="2"/>
       <c r="G48" s="1">
@@ -9251,23 +9254,23 @@
         <v>1</v>
       </c>
       <c r="W48" s="1">
-        <v>2000.0</v>
+        <v>0</v>
       </c>
       <c r="X48" s="2">
         <v>0.01</v>
       </c>
       <c r="Y48" s="1">
-        <v>-2000.0</v>
+        <v>-24000.0</v>
       </c>
       <c r="Z48" s="2"/>
       <c r="AA48" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AB48" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AC48" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AD48">
         <v>0</v>
@@ -9289,7 +9292,7 @@
       </c>
       <c r="D49" s="2"/>
       <c r="E49" s="5">
-        <v>2000.0</v>
+        <v>24000.0</v>
       </c>
       <c r="F49" s="2"/>
       <c r="G49" s="1">
@@ -9323,23 +9326,23 @@
         <v>1</v>
       </c>
       <c r="W49" s="1">
-        <v>2000.0</v>
+        <v>0</v>
       </c>
       <c r="X49" s="2">
         <v>0.01</v>
       </c>
       <c r="Y49" s="1">
-        <v>-2000.0</v>
+        <v>-24000.0</v>
       </c>
       <c r="Z49" s="2"/>
       <c r="AA49" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AB49" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AC49" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AD49">
         <v>0</v>
@@ -9361,7 +9364,7 @@
       </c>
       <c r="D50" s="2"/>
       <c r="E50" s="5">
-        <v>2000.0</v>
+        <v>24000.0</v>
       </c>
       <c r="F50" s="2"/>
       <c r="G50" s="1">
@@ -9395,23 +9398,23 @@
         <v>1</v>
       </c>
       <c r="W50" s="1">
-        <v>2000.0</v>
+        <v>0</v>
       </c>
       <c r="X50" s="2">
         <v>0.01</v>
       </c>
       <c r="Y50" s="1">
-        <v>-2000.0</v>
+        <v>-24000.0</v>
       </c>
       <c r="Z50" s="2"/>
       <c r="AA50" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AB50" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AC50" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AD50">
         <v>0</v>
@@ -9433,7 +9436,7 @@
       </c>
       <c r="D51" s="2"/>
       <c r="E51" s="5">
-        <v>2000.0</v>
+        <v>24000.0</v>
       </c>
       <c r="F51" s="2"/>
       <c r="G51" s="1">
@@ -9467,23 +9470,23 @@
         <v>1</v>
       </c>
       <c r="W51" s="1">
-        <v>2000.0</v>
+        <v>0</v>
       </c>
       <c r="X51" s="2">
         <v>0.01</v>
       </c>
       <c r="Y51" s="1">
-        <v>-2000.0</v>
+        <v>-24000.0</v>
       </c>
       <c r="Z51" s="2"/>
       <c r="AA51" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AB51" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AC51" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AD51">
         <v>0</v>
@@ -9505,7 +9508,7 @@
       </c>
       <c r="D52" s="2"/>
       <c r="E52" s="5">
-        <v>2000.0</v>
+        <v>24000.0</v>
       </c>
       <c r="F52" s="2"/>
       <c r="G52" s="1">
@@ -9539,23 +9542,23 @@
         <v>1</v>
       </c>
       <c r="W52" s="1">
-        <v>2000.0</v>
+        <v>0</v>
       </c>
       <c r="X52" s="2">
         <v>0.01</v>
       </c>
       <c r="Y52" s="1">
-        <v>-2000.0</v>
+        <v>-24000.0</v>
       </c>
       <c r="Z52" s="2"/>
       <c r="AA52" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AB52" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AC52" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AD52">
         <v>0</v>
@@ -9577,7 +9580,7 @@
       </c>
       <c r="D53" s="14"/>
       <c r="E53" s="13">
-        <v>2000.0</v>
+        <v>24000.0</v>
       </c>
       <c r="F53" s="14"/>
       <c r="G53" s="13">
@@ -9611,23 +9614,23 @@
         <v>1</v>
       </c>
       <c r="W53" s="13">
-        <v>2000.0</v>
+        <v>0</v>
       </c>
       <c r="X53" s="14">
         <v>0.01</v>
       </c>
       <c r="Y53" s="13">
-        <v>-2000.0</v>
+        <v>-24000.0</v>
       </c>
       <c r="Z53" s="14"/>
       <c r="AA53" s="13">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AB53" s="13">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AC53" s="13">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AD53" s="3">
         <v>0</v>
@@ -9650,7 +9653,7 @@
       </c>
       <c r="D54" s="2"/>
       <c r="E54" s="5">
-        <v>2000.0</v>
+        <v>24000.0</v>
       </c>
       <c r="F54" s="2"/>
       <c r="G54" s="1">
@@ -9684,23 +9687,23 @@
         <v>1</v>
       </c>
       <c r="W54" s="1">
-        <v>2000.0</v>
+        <v>0</v>
       </c>
       <c r="X54" s="2">
         <v>0.01</v>
       </c>
       <c r="Y54" s="1">
-        <v>-2000.0</v>
+        <v>-24000.0</v>
       </c>
       <c r="Z54" s="2"/>
       <c r="AA54" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AB54" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AC54" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AD54">
         <v>0</v>
@@ -9722,7 +9725,7 @@
       </c>
       <c r="D55" s="2"/>
       <c r="E55" s="5">
-        <v>2000.0</v>
+        <v>24000.0</v>
       </c>
       <c r="F55" s="2"/>
       <c r="G55" s="1">
@@ -9756,23 +9759,23 @@
         <v>1</v>
       </c>
       <c r="W55" s="1">
-        <v>2000.0</v>
+        <v>0</v>
       </c>
       <c r="X55" s="2">
         <v>0.01</v>
       </c>
       <c r="Y55" s="1">
-        <v>-2000.0</v>
+        <v>-24000.0</v>
       </c>
       <c r="Z55" s="2"/>
       <c r="AA55" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AB55" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AC55" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AD55">
         <v>0</v>
@@ -9794,7 +9797,7 @@
       </c>
       <c r="D56" s="2"/>
       <c r="E56" s="5">
-        <v>2000.0</v>
+        <v>24000.0</v>
       </c>
       <c r="F56" s="2"/>
       <c r="G56" s="1">
@@ -9828,23 +9831,23 @@
         <v>1</v>
       </c>
       <c r="W56" s="1">
-        <v>2000.0</v>
+        <v>0</v>
       </c>
       <c r="X56" s="2">
         <v>0.01</v>
       </c>
       <c r="Y56" s="1">
-        <v>-2000.0</v>
+        <v>-24000.0</v>
       </c>
       <c r="Z56" s="2"/>
       <c r="AA56" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AB56" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AC56" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AD56">
         <v>0</v>
@@ -9866,7 +9869,7 @@
       </c>
       <c r="D57" s="14"/>
       <c r="E57" s="13">
-        <v>2000.0</v>
+        <v>24000.0</v>
       </c>
       <c r="F57" s="14"/>
       <c r="G57" s="13">
@@ -9900,23 +9903,23 @@
         <v>1</v>
       </c>
       <c r="W57" s="13">
-        <v>2000.0</v>
+        <v>0</v>
       </c>
       <c r="X57" s="14">
         <v>0.01</v>
       </c>
       <c r="Y57" s="13">
-        <v>-2000.0</v>
+        <v>-24000.0</v>
       </c>
       <c r="Z57" s="14"/>
       <c r="AA57" s="13">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AB57" s="13">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AC57" s="13">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AD57" s="3">
         <v>0</v>
@@ -9939,7 +9942,7 @@
       </c>
       <c r="D58" s="2"/>
       <c r="E58" s="5">
-        <v>2000.0</v>
+        <v>24000.0</v>
       </c>
       <c r="F58" s="2"/>
       <c r="G58" s="1">
@@ -9973,23 +9976,23 @@
         <v>1</v>
       </c>
       <c r="W58" s="1">
-        <v>2000.0</v>
+        <v>0</v>
       </c>
       <c r="X58" s="2">
         <v>0.01</v>
       </c>
       <c r="Y58" s="1">
-        <v>-2000.0</v>
+        <v>-24000.0</v>
       </c>
       <c r="Z58" s="2"/>
       <c r="AA58" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AB58" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AC58" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AD58">
         <v>0</v>
@@ -10011,7 +10014,7 @@
       </c>
       <c r="D59" s="2"/>
       <c r="E59" s="5">
-        <v>2000.0</v>
+        <v>24000.0</v>
       </c>
       <c r="F59" s="2"/>
       <c r="G59" s="1">
@@ -10045,23 +10048,23 @@
         <v>1</v>
       </c>
       <c r="W59" s="1">
-        <v>2000.0</v>
+        <v>0</v>
       </c>
       <c r="X59" s="2">
         <v>0.01</v>
       </c>
       <c r="Y59" s="1">
-        <v>-2000.0</v>
+        <v>-24000.0</v>
       </c>
       <c r="Z59" s="2"/>
       <c r="AA59" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AB59" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AC59" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AD59">
         <v>0</v>
@@ -10083,7 +10086,7 @@
       </c>
       <c r="D60" s="2"/>
       <c r="E60" s="5">
-        <v>2000.0</v>
+        <v>24000.0</v>
       </c>
       <c r="F60" s="2"/>
       <c r="G60" s="1">
@@ -10117,23 +10120,23 @@
         <v>1</v>
       </c>
       <c r="W60" s="1">
-        <v>2000.0</v>
+        <v>0</v>
       </c>
       <c r="X60" s="2">
         <v>0.01</v>
       </c>
       <c r="Y60" s="1">
-        <v>-2000.0</v>
+        <v>-24000.0</v>
       </c>
       <c r="Z60" s="2"/>
       <c r="AA60" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AB60" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AC60" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AD60">
         <v>0</v>
@@ -10155,7 +10158,7 @@
       </c>
       <c r="D61" s="2"/>
       <c r="E61" s="5">
-        <v>2000.0</v>
+        <v>24000.0</v>
       </c>
       <c r="F61" s="2"/>
       <c r="G61" s="1">
@@ -10189,23 +10192,23 @@
         <v>1</v>
       </c>
       <c r="W61" s="1">
-        <v>2000.0</v>
+        <v>0</v>
       </c>
       <c r="X61" s="2">
         <v>0.01</v>
       </c>
       <c r="Y61" s="1">
-        <v>-2000.0</v>
+        <v>-24000.0</v>
       </c>
       <c r="Z61" s="2"/>
       <c r="AA61" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AB61" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AC61" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AD61">
         <v>0</v>
@@ -10227,7 +10230,7 @@
       </c>
       <c r="D62" s="2"/>
       <c r="E62" s="5">
-        <v>2000.0</v>
+        <v>24000.0</v>
       </c>
       <c r="F62" s="2"/>
       <c r="G62" s="1">
@@ -10261,23 +10264,23 @@
         <v>1</v>
       </c>
       <c r="W62" s="1">
-        <v>2000.0</v>
+        <v>0</v>
       </c>
       <c r="X62" s="2">
         <v>0.01</v>
       </c>
       <c r="Y62" s="1">
-        <v>-2000.0</v>
+        <v>-24000.0</v>
       </c>
       <c r="Z62" s="2"/>
       <c r="AA62" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AB62" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AC62" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AD62">
         <v>0</v>
@@ -10299,7 +10302,7 @@
       </c>
       <c r="D63" s="2"/>
       <c r="E63" s="5">
-        <v>2000.0</v>
+        <v>24000.0</v>
       </c>
       <c r="F63" s="2"/>
       <c r="G63" s="1">
@@ -10333,23 +10336,23 @@
         <v>1</v>
       </c>
       <c r="W63" s="1">
-        <v>2000.0</v>
+        <v>0</v>
       </c>
       <c r="X63" s="2">
         <v>0.01</v>
       </c>
       <c r="Y63" s="1">
-        <v>-2000.0</v>
+        <v>-24000.0</v>
       </c>
       <c r="Z63" s="2"/>
       <c r="AA63" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AB63" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AC63" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AD63">
         <v>0</v>
@@ -10371,7 +10374,7 @@
       </c>
       <c r="D64" s="2"/>
       <c r="E64" s="5">
-        <v>2000.0</v>
+        <v>24000.0</v>
       </c>
       <c r="F64" s="2"/>
       <c r="G64" s="1">
@@ -10405,23 +10408,23 @@
         <v>1</v>
       </c>
       <c r="W64" s="1">
-        <v>2000.0</v>
+        <v>0</v>
       </c>
       <c r="X64" s="2">
         <v>0.01</v>
       </c>
       <c r="Y64" s="1">
-        <v>-2000.0</v>
+        <v>-24000.0</v>
       </c>
       <c r="Z64" s="2"/>
       <c r="AA64" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AB64" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AC64" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AD64">
         <v>0</v>
@@ -10443,7 +10446,7 @@
       </c>
       <c r="D65" s="2"/>
       <c r="E65" s="5">
-        <v>2000.0</v>
+        <v>24000.0</v>
       </c>
       <c r="F65" s="2"/>
       <c r="G65" s="1">
@@ -10477,23 +10480,23 @@
         <v>1</v>
       </c>
       <c r="W65" s="1">
-        <v>2000.0</v>
+        <v>0</v>
       </c>
       <c r="X65" s="2">
         <v>0.01</v>
       </c>
       <c r="Y65" s="1">
-        <v>-2000.0</v>
+        <v>-24000.0</v>
       </c>
       <c r="Z65" s="2"/>
       <c r="AA65" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AB65" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AC65" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AD65">
         <v>0</v>
@@ -10515,7 +10518,7 @@
       </c>
       <c r="D66" s="2"/>
       <c r="E66" s="5">
-        <v>2000.0</v>
+        <v>24000.0</v>
       </c>
       <c r="F66" s="2"/>
       <c r="G66" s="1">
@@ -10549,23 +10552,23 @@
         <v>1</v>
       </c>
       <c r="W66" s="1">
-        <v>2000.0</v>
+        <v>0</v>
       </c>
       <c r="X66" s="2">
         <v>0.01</v>
       </c>
       <c r="Y66" s="1">
-        <v>-2000.0</v>
+        <v>-24000.0</v>
       </c>
       <c r="Z66" s="2"/>
       <c r="AA66" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AB66" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AC66" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AD66">
         <v>0</v>
@@ -10587,7 +10590,7 @@
       </c>
       <c r="D67" s="2"/>
       <c r="E67" s="5">
-        <v>2000.0</v>
+        <v>24000.0</v>
       </c>
       <c r="F67" s="2"/>
       <c r="G67" s="1">
@@ -10621,23 +10624,23 @@
         <v>1</v>
       </c>
       <c r="W67" s="1">
-        <v>2000.0</v>
+        <v>0</v>
       </c>
       <c r="X67" s="2">
         <v>0.01</v>
       </c>
       <c r="Y67" s="1">
-        <v>-2000.0</v>
+        <v>-24000.0</v>
       </c>
       <c r="Z67" s="2"/>
       <c r="AA67" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AB67" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AC67" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AD67">
         <v>0</v>
@@ -10659,7 +10662,7 @@
       </c>
       <c r="D68" s="2"/>
       <c r="E68" s="5">
-        <v>2000.0</v>
+        <v>24000.0</v>
       </c>
       <c r="F68" s="2"/>
       <c r="G68" s="1">
@@ -10693,23 +10696,23 @@
         <v>1</v>
       </c>
       <c r="W68" s="1">
-        <v>2000.0</v>
+        <v>0</v>
       </c>
       <c r="X68" s="2">
         <v>0.01</v>
       </c>
       <c r="Y68" s="1">
-        <v>-2000.0</v>
+        <v>-24000.0</v>
       </c>
       <c r="Z68" s="2"/>
       <c r="AA68" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AB68" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AC68" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AD68">
         <v>0</v>
@@ -10731,7 +10734,7 @@
       </c>
       <c r="D69" s="2"/>
       <c r="E69" s="5">
-        <v>2000.0</v>
+        <v>24000.0</v>
       </c>
       <c r="F69" s="2"/>
       <c r="G69" s="1">
@@ -10765,23 +10768,23 @@
         <v>1</v>
       </c>
       <c r="W69" s="1">
-        <v>2000.0</v>
+        <v>0</v>
       </c>
       <c r="X69" s="2">
         <v>0.01</v>
       </c>
       <c r="Y69" s="1">
-        <v>-2000.0</v>
+        <v>-24000.0</v>
       </c>
       <c r="Z69" s="2"/>
       <c r="AA69" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AB69" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AC69" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AD69">
         <v>0</v>
@@ -10803,7 +10806,7 @@
       </c>
       <c r="D70" s="2"/>
       <c r="E70" s="5">
-        <v>2000.0</v>
+        <v>24000.0</v>
       </c>
       <c r="F70" s="2"/>
       <c r="G70" s="1">
@@ -10837,23 +10840,23 @@
         <v>1</v>
       </c>
       <c r="W70" s="1">
-        <v>2000.0</v>
+        <v>0</v>
       </c>
       <c r="X70" s="2">
         <v>0.01</v>
       </c>
       <c r="Y70" s="1">
-        <v>-2000.0</v>
+        <v>-24000.0</v>
       </c>
       <c r="Z70" s="2"/>
       <c r="AA70" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AB70" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AC70" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AD70">
         <v>0</v>
@@ -10875,7 +10878,7 @@
       </c>
       <c r="D71" s="2"/>
       <c r="E71" s="5">
-        <v>2000.0</v>
+        <v>24000.0</v>
       </c>
       <c r="F71" s="2"/>
       <c r="G71" s="1">
@@ -10909,23 +10912,23 @@
         <v>1</v>
       </c>
       <c r="W71" s="1">
-        <v>2000.0</v>
+        <v>0</v>
       </c>
       <c r="X71" s="2">
         <v>0.01</v>
       </c>
       <c r="Y71" s="1">
-        <v>-2000.0</v>
+        <v>-24000.0</v>
       </c>
       <c r="Z71" s="2"/>
       <c r="AA71" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AB71" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AC71" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AD71">
         <v>0</v>
@@ -10947,7 +10950,7 @@
       </c>
       <c r="D72" s="16"/>
       <c r="E72" s="5">
-        <v>2000.0</v>
+        <v>24000.0</v>
       </c>
       <c r="F72" s="16"/>
       <c r="G72" s="5">
@@ -10981,23 +10984,23 @@
         <v>1</v>
       </c>
       <c r="W72" s="5">
-        <v>2000.0</v>
+        <v>0</v>
       </c>
       <c r="X72" s="16">
         <v>0.01</v>
       </c>
       <c r="Y72" s="5">
-        <v>-2000.0</v>
+        <v>-24000.0</v>
       </c>
       <c r="Z72" s="16"/>
       <c r="AA72" s="5">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AB72" s="5">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AC72" s="5">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AD72" s="15">
         <v>0</v>
@@ -11269,14 +11272,574 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:C72"/>
   <sheetViews>
     <sheetView tabSelected="0" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
-  <sheetData/>
+  <sheetData>
+    <row r="5" spans="1:3">
+      <c r="B5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C5" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6">
+        <v>1991</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7">
+        <v>1992</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8">
+        <v>1993</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9">
+        <v>1994</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10">
+        <v>1995</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11">
+        <v>1996</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12">
+        <v>1997</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13">
+        <v>1998</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14">
+        <v>1999</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16">
+        <v>2001</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17">
+        <v>2002</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18">
+        <v>2003</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19">
+        <v>2004</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20">
+        <v>2005</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21">
+        <v>2006</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22">
+        <v>2007</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23">
+        <v>2008</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24">
+        <v>2009</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25">
+        <v>2010</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26">
+        <v>2011</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27">
+        <v>2012</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28">
+        <v>2013</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="A30">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="A31">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
+      <c r="A32">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
+      <c r="A33">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="A34">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
+      <c r="A35">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="A36">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3">
+      <c r="A37">
+        <v>2022</v>
+      </c>
+      <c r="B37">
+        <v>100.0</v>
+      </c>
+      <c r="C37">
+        <v>100.0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3">
+      <c r="A38">
+        <v>2023</v>
+      </c>
+      <c r="B38">
+        <v>100.0</v>
+      </c>
+      <c r="C38">
+        <v>100.0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3">
+      <c r="A39">
+        <v>2024</v>
+      </c>
+      <c r="B39">
+        <v>100.0</v>
+      </c>
+      <c r="C39">
+        <v>100.0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3">
+      <c r="A40">
+        <v>2025</v>
+      </c>
+      <c r="B40">
+        <v>100.0</v>
+      </c>
+      <c r="C40">
+        <v>100.0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3">
+      <c r="A41">
+        <v>2026</v>
+      </c>
+      <c r="B41">
+        <v>100.0</v>
+      </c>
+      <c r="C41">
+        <v>100.0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3">
+      <c r="A42">
+        <v>2027</v>
+      </c>
+      <c r="B42">
+        <v>100.0</v>
+      </c>
+      <c r="C42">
+        <v>100.0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3">
+      <c r="A43">
+        <v>2028</v>
+      </c>
+      <c r="B43">
+        <v>100.0</v>
+      </c>
+      <c r="C43">
+        <v>100.0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3">
+      <c r="A44">
+        <v>2029</v>
+      </c>
+      <c r="B44">
+        <v>100.0</v>
+      </c>
+      <c r="C44">
+        <v>100.0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3">
+      <c r="A45">
+        <v>2030</v>
+      </c>
+      <c r="B45">
+        <v>100.0</v>
+      </c>
+      <c r="C45">
+        <v>100.0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3">
+      <c r="A46">
+        <v>2031</v>
+      </c>
+      <c r="B46">
+        <v>100.0</v>
+      </c>
+      <c r="C46">
+        <v>100.0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3">
+      <c r="A47">
+        <v>2032</v>
+      </c>
+      <c r="B47">
+        <v>100.0</v>
+      </c>
+      <c r="C47">
+        <v>100.0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3">
+      <c r="A48">
+        <v>2033</v>
+      </c>
+      <c r="B48">
+        <v>100.0</v>
+      </c>
+      <c r="C48">
+        <v>100.0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3">
+      <c r="A49">
+        <v>2034</v>
+      </c>
+      <c r="B49">
+        <v>100.0</v>
+      </c>
+      <c r="C49">
+        <v>100.0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3">
+      <c r="A50">
+        <v>2035</v>
+      </c>
+      <c r="B50">
+        <v>100.0</v>
+      </c>
+      <c r="C50">
+        <v>100.0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3">
+      <c r="A51">
+        <v>2036</v>
+      </c>
+      <c r="B51">
+        <v>100.0</v>
+      </c>
+      <c r="C51">
+        <v>100.0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3">
+      <c r="A52">
+        <v>2037</v>
+      </c>
+      <c r="B52">
+        <v>100.0</v>
+      </c>
+      <c r="C52">
+        <v>100.0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3">
+      <c r="A53">
+        <v>2038</v>
+      </c>
+      <c r="B53">
+        <v>100.0</v>
+      </c>
+      <c r="C53">
+        <v>100.0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3">
+      <c r="A54">
+        <v>2039</v>
+      </c>
+      <c r="B54">
+        <v>100.0</v>
+      </c>
+      <c r="C54">
+        <v>100.0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3">
+      <c r="A55">
+        <v>2040</v>
+      </c>
+      <c r="B55">
+        <v>100.0</v>
+      </c>
+      <c r="C55">
+        <v>100.0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3">
+      <c r="A56">
+        <v>2041</v>
+      </c>
+      <c r="B56">
+        <v>100.0</v>
+      </c>
+      <c r="C56">
+        <v>100.0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3">
+      <c r="A57">
+        <v>2042</v>
+      </c>
+      <c r="B57">
+        <v>100.0</v>
+      </c>
+      <c r="C57">
+        <v>100.0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3">
+      <c r="A58">
+        <v>2043</v>
+      </c>
+      <c r="B58">
+        <v>100.0</v>
+      </c>
+      <c r="C58">
+        <v>100.0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3">
+      <c r="A59">
+        <v>2044</v>
+      </c>
+      <c r="B59">
+        <v>100.0</v>
+      </c>
+      <c r="C59">
+        <v>100.0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3">
+      <c r="A60">
+        <v>2045</v>
+      </c>
+      <c r="B60">
+        <v>100.0</v>
+      </c>
+      <c r="C60">
+        <v>100.0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3">
+      <c r="A61">
+        <v>2046</v>
+      </c>
+      <c r="B61">
+        <v>100.0</v>
+      </c>
+      <c r="C61">
+        <v>100.0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3">
+      <c r="A62">
+        <v>2047</v>
+      </c>
+      <c r="B62">
+        <v>100.0</v>
+      </c>
+      <c r="C62">
+        <v>100.0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3">
+      <c r="A63">
+        <v>2048</v>
+      </c>
+      <c r="B63">
+        <v>100.0</v>
+      </c>
+      <c r="C63">
+        <v>100.0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3">
+      <c r="A64">
+        <v>2049</v>
+      </c>
+      <c r="B64">
+        <v>100.0</v>
+      </c>
+      <c r="C64">
+        <v>100.0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3">
+      <c r="A65">
+        <v>2050</v>
+      </c>
+      <c r="B65">
+        <v>100.0</v>
+      </c>
+      <c r="C65">
+        <v>100.0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3">
+      <c r="A66">
+        <v>2051</v>
+      </c>
+      <c r="B66">
+        <v>100.0</v>
+      </c>
+      <c r="C66">
+        <v>100.0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3">
+      <c r="A67">
+        <v>2052</v>
+      </c>
+      <c r="B67">
+        <v>100.0</v>
+      </c>
+      <c r="C67">
+        <v>100.0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3">
+      <c r="A68">
+        <v>2053</v>
+      </c>
+      <c r="B68">
+        <v>100.0</v>
+      </c>
+      <c r="C68">
+        <v>100.0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3">
+      <c r="A69">
+        <v>2054</v>
+      </c>
+      <c r="B69">
+        <v>100.0</v>
+      </c>
+      <c r="C69">
+        <v>100.0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3">
+      <c r="A70">
+        <v>2055</v>
+      </c>
+      <c r="B70">
+        <v>100.0</v>
+      </c>
+      <c r="C70">
+        <v>100.0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3">
+      <c r="A71">
+        <v>2056</v>
+      </c>
+      <c r="B71">
+        <v>100.0</v>
+      </c>
+      <c r="C71">
+        <v>100.0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3">
+      <c r="A72">
+        <v>2057</v>
+      </c>
+      <c r="B72">
+        <v>100.0</v>
+      </c>
+      <c r="C72">
+        <v>100.0</v>
+      </c>
+    </row>
+  </sheetData>
   <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="1" orientation="default" scale="100" fitToHeight="1" fitToWidth="1" pageOrder="downThenOver"/>

</xml_diff>